<commit_message>
Added option to reject 10% of the outliers
</commit_message>
<xml_diff>
--- a/features/original.xlsx
+++ b/features/original.xlsx
@@ -471,7 +471,7 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>center_mass</t>
+          <t>barycentre_distance</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
@@ -519,10 +519,8 @@
           <t>testModels/db/0/m0/m0.off</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>[0.3338  0.27524 0.39134]</t>
-        </is>
+      <c r="I2" t="n">
+        <v>0.5833692785551206</v>
       </c>
       <c r="J2" t="n">
         <v>0.30655993840855</v>
@@ -563,10 +561,8 @@
           <t>testModels/db/0/m1/m1.off</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>[0.22685 0.21716 0.32942]</t>
-        </is>
+      <c r="I3" t="n">
+        <v>0.4551239187853133</v>
       </c>
       <c r="J3" t="n">
         <v>0.13669153135125</v>
@@ -607,10 +603,8 @@
           <t>testModels/db/0/m2/m2.off</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>[0.32096 0.26085 0.36399]</t>
-        </is>
+      <c r="I4" t="n">
+        <v>0.5509480836102678</v>
       </c>
       <c r="J4" t="n">
         <v>0.2757459366555</v>
@@ -651,10 +645,8 @@
           <t>testModels/db/0/m3/m3.off</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>[0.4796  0.31391 0.42554]</t>
-        </is>
+      <c r="I5" t="n">
+        <v>0.7138964227799601</v>
       </c>
       <c r="J5" t="n">
         <v>0.4575223871524</v>
@@ -695,10 +687,8 @@
           <t>testModels/db/0/m4/m4.off</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>[ 0.12036 -0.70121 -0.08675]</t>
-        </is>
+      <c r="I6" t="n">
+        <v>0.7167299028897499</v>
       </c>
       <c r="J6" t="n">
         <v>0.15520719289875</v>
@@ -739,10 +729,8 @@
           <t>testModels/db/0/m5/m5.off</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>[0.31276 0.28692 0.40863]</t>
-        </is>
+      <c r="I7" t="n">
+        <v>0.5891684456837839</v>
       </c>
       <c r="J7" t="n">
         <v>0.2412601344584</v>
@@ -783,10 +771,8 @@
           <t>testModels/db/0/m6/m6.off</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>[0.34655 0.47303 0.44325]</t>
-        </is>
+      <c r="I8" t="n">
+        <v>0.7350670881757851</v>
       </c>
       <c r="J8" t="n">
         <v>0.4137792986902</v>
@@ -827,10 +813,8 @@
           <t>testModels/db/0/m7/m7.off</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>[0.2996  0.37981 0.47358]</t>
-        </is>
+      <c r="I9" t="n">
+        <v>0.6769725559850669</v>
       </c>
       <c r="J9" t="n">
         <v>0.2864681436477</v>
@@ -871,10 +855,8 @@
           <t>testModels/db/0/m8/m8.off</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>[0.26053 0.51883 0.38664]</t>
-        </is>
+      <c r="I10" t="n">
+        <v>0.6975254655816926</v>
       </c>
       <c r="J10" t="n">
         <v>0.3486246117801</v>
@@ -915,10 +897,8 @@
           <t>testModels/db/0/m9/m9.off</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>[ 0.50194 11.04056  0.43287]</t>
-        </is>
+      <c r="I11" t="n">
+        <v>11.0604390210595</v>
       </c>
       <c r="J11" t="n">
         <v>0.35013334705725</v>
@@ -959,10 +939,8 @@
           <t>testModels/db/1/m100/m100.off</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>[0.2914  0.2242  0.49578]</t>
-        </is>
+      <c r="I12" t="n">
+        <v>0.617230475763601</v>
       </c>
       <c r="J12" t="n">
         <v>0.21949979381205</v>
@@ -1003,10 +981,8 @@
           <t>testModels/db/1/m101/m101.off</t>
         </is>
       </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>[0.21684 0.47747 0.70053]</t>
-        </is>
+      <c r="I13" t="n">
+        <v>0.8750635992922768</v>
       </c>
       <c r="J13" t="n">
         <v>0.2406917928752999</v>
@@ -1047,10 +1023,8 @@
           <t>testModels/db/1/m102/m102.off</t>
         </is>
       </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>[0.21525 0.26477 0.46865]</t>
-        </is>
+      <c r="I14" t="n">
+        <v>0.5797146577155331</v>
       </c>
       <c r="J14" t="n">
         <v>0.1520326298799</v>
@@ -1091,10 +1065,8 @@
           <t>testModels/db/1/m103/m103.off</t>
         </is>
       </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>[0.1426  0.62842 0.43926]</t>
-        </is>
+      <c r="I15" t="n">
+        <v>0.7798726009303663</v>
       </c>
       <c r="J15" t="n">
         <v>0.14984652717595</v>
@@ -1135,10 +1107,8 @@
           <t>testModels/db/1/m104/m104.off</t>
         </is>
       </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>[0.49539 0.47059 0.15403]</t>
-        </is>
+      <c r="I16" t="n">
+        <v>0.7004238388061579</v>
       </c>
       <c r="J16" t="n">
         <v>0.1849215228111</v>
@@ -1179,10 +1149,8 @@
           <t>testModels/db/1/m105/m105.off</t>
         </is>
       </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>[0.15    0.5408  0.45165]</t>
-        </is>
+      <c r="I17" t="n">
+        <v>0.720381260007417</v>
       </c>
       <c r="J17" t="n">
         <v>0.21408164502945</v>
@@ -1223,10 +1191,8 @@
           <t>testModels/db/1/m106/m106.off</t>
         </is>
       </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>[0.12361 0.38183 0.59404]</t>
-        </is>
+      <c r="I18" t="n">
+        <v>0.7169114809430549</v>
       </c>
       <c r="J18" t="n">
         <v>0.11349285504</v>
@@ -1267,10 +1233,8 @@
           <t>testModels/db/1/m107/m107.off</t>
         </is>
       </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>[0.14444 0.52042 0.45173]</t>
-        </is>
+      <c r="I19" t="n">
+        <v>0.7041051577722928</v>
       </c>
       <c r="J19" t="n">
         <v>0.1958584251483</v>
@@ -1311,10 +1275,8 @@
           <t>testModels/db/1/m108/m108.off</t>
         </is>
       </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>[0.57152 0.5199  0.15692]</t>
-        </is>
+      <c r="I20" t="n">
+        <v>0.7883864757508037</v>
       </c>
       <c r="J20" t="n">
         <v>0.2158320410406</v>
@@ -1355,10 +1317,8 @@
           <t>testModels/db/1/m109/m109.off</t>
         </is>
       </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>[0.39722 0.31741 0.24988]</t>
-        </is>
+      <c r="I21" t="n">
+        <v>0.5665445074166562</v>
       </c>
       <c r="J21" t="n">
         <v>0.3382912707369999</v>
@@ -1399,10 +1359,8 @@
           <t>testModels/db/1/m110/m110.off</t>
         </is>
       </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>[0.24707 0.31258 0.44098]</t>
-        </is>
+      <c r="I22" t="n">
+        <v>0.5943193461023402</v>
       </c>
       <c r="J22" t="n">
         <v>0.2939200007275</v>
@@ -1443,10 +1401,8 @@
           <t>testModels/db/1/m111/m111.off</t>
         </is>
       </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>[0.21977 0.3188  0.42829]</t>
-        </is>
+      <c r="I23" t="n">
+        <v>0.5773744061375005</v>
       </c>
       <c r="J23" t="n">
         <v>0.24167553026045</v>
@@ -1487,10 +1443,8 @@
           <t>testModels/db/1/m112/m112.off</t>
         </is>
       </c>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>[0.45673 0.63818 0.30562]</t>
-        </is>
+      <c r="I24" t="n">
+        <v>0.8421914177505204</v>
       </c>
       <c r="J24" t="n">
         <v>0.5465292191511999</v>
@@ -1531,10 +1485,8 @@
           <t>testModels/db/10/m1000/m1000.off</t>
         </is>
       </c>
-      <c r="I25" t="inlineStr">
-        <is>
-          <t>[ 0.50971 -0.60521  0.48632]</t>
-        </is>
+      <c r="I25" t="n">
+        <v>0.9287522775164535</v>
       </c>
       <c r="J25" t="n">
         <v>0.6396504912319999</v>
@@ -1575,10 +1527,8 @@
           <t>testModels/db/10/m1001/m1001.off</t>
         </is>
       </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>[0.35437 0.26538 0.3536 ]</t>
-        </is>
+      <c r="I26" t="n">
+        <v>0.5665998934600771</v>
       </c>
       <c r="J26" t="n">
         <v>0.36339438</v>
@@ -1619,10 +1569,8 @@
           <t>testModels/db/10/m1002/m1002.off</t>
         </is>
       </c>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>[  0.93078 -36.67351   2.3422 ]</t>
-        </is>
+      <c r="I27" t="n">
+        <v>36.76001108224993</v>
       </c>
       <c r="J27" t="n">
         <v>0.6687993559893</v>
@@ -1663,10 +1611,8 @@
           <t>testModels/db/10/m1003/m1003.off</t>
         </is>
       </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>[0.45072 2.7656  0.39009]</t>
-        </is>
+      <c r="I28" t="n">
+        <v>2.829112919506064</v>
       </c>
       <c r="J28" t="n">
         <v>0.8344160736335999</v>
@@ -1707,10 +1653,8 @@
           <t>testModels/db/10/m1004/m1004.off</t>
         </is>
       </c>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>[0.38301 1.54942 0.11717]</t>
-        </is>
+      <c r="I29" t="n">
+        <v>1.60035386373809</v>
       </c>
       <c r="J29" t="n">
         <v>0.58610156302355</v>
@@ -1751,10 +1695,8 @@
           <t>testModels/db/10/m1005/m1005.off</t>
         </is>
       </c>
-      <c r="I30" t="inlineStr">
-        <is>
-          <t>[ 0.25235 -3.02591  0.25488]</t>
-        </is>
+      <c r="I30" t="n">
+        <v>3.047092386015169</v>
       </c>
       <c r="J30" t="n">
         <v>0.20376973537075</v>
@@ -1795,10 +1737,8 @@
           <t>testModels/db/10/m1006/m1006.off</t>
         </is>
       </c>
-      <c r="I31" t="inlineStr">
-        <is>
-          <t>[0.6961  1.57667 0.74224]</t>
-        </is>
+      <c r="I31" t="n">
+        <v>1.876525832695281</v>
       </c>
       <c r="J31" t="n">
         <v>0.4711576637420999</v>
@@ -1839,10 +1779,8 @@
           <t>testModels/db/10/m1007/m1007.off</t>
         </is>
       </c>
-      <c r="I32" t="inlineStr">
-        <is>
-          <t>[  0.64605 -14.89311  -1.04891]</t>
-        </is>
+      <c r="I32" t="n">
+        <v>14.94397686443064</v>
       </c>
       <c r="J32" t="n">
         <v>0.50159135133015</v>
@@ -1883,10 +1821,8 @@
           <t>testModels/db/10/m1008/m1008.off</t>
         </is>
       </c>
-      <c r="I33" t="inlineStr">
-        <is>
-          <t>[ 0.37225 -0.08517  0.25697]</t>
-        </is>
+      <c r="I33" t="n">
+        <v>0.4602829826751681</v>
       </c>
       <c r="J33" t="n">
         <v>0.6686612839449999</v>
@@ -1927,10 +1863,8 @@
           <t>testModels/db/10/m1009/m1009.off</t>
         </is>
       </c>
-      <c r="I34" t="inlineStr">
-        <is>
-          <t>[ 0.35391 -2.25266  0.38447]</t>
-        </is>
+      <c r="I34" t="n">
+        <v>2.312477163242846</v>
       </c>
       <c r="J34" t="n">
         <v>0.3602333179622</v>
@@ -1971,10 +1905,8 @@
           <t>testModels/db/10/m1010/m1010.off</t>
         </is>
       </c>
-      <c r="I35" t="inlineStr">
-        <is>
-          <t>[0.50137 2.125   0.39554]</t>
-        </is>
+      <c r="I35" t="n">
+        <v>2.218883589454054</v>
       </c>
       <c r="J35" t="n">
         <v>0.4932343272991999</v>
@@ -2015,10 +1947,8 @@
           <t>testModels/db/10/m1011/m1011.off</t>
         </is>
       </c>
-      <c r="I36" t="inlineStr">
-        <is>
-          <t>[ 0.46551 -1.25139  0.42539]</t>
-        </is>
+      <c r="I36" t="n">
+        <v>1.40129883032089</v>
       </c>
       <c r="J36" t="n">
         <v>0.66857728021875</v>
@@ -2059,10 +1989,8 @@
           <t>testModels/db/10/m1012/m1012.off</t>
         </is>
       </c>
-      <c r="I37" t="inlineStr">
-        <is>
-          <t>[ 0.04165 -6.66756  0.6309 ]</t>
-        </is>
+      <c r="I37" t="n">
+        <v>6.697467331631407</v>
       </c>
       <c r="J37" t="n">
         <v>0.4852904050862999</v>
@@ -2103,10 +2031,8 @@
           <t>testModels/db/11/m1100/m1100.off</t>
         </is>
       </c>
-      <c r="I38" t="inlineStr">
-        <is>
-          <t>[0.12992 0.49669 0.15885]</t>
-        </is>
+      <c r="I38" t="n">
+        <v>0.5374154606745417</v>
       </c>
       <c r="J38" t="n">
         <v>0.0358110831519</v>
@@ -2147,10 +2073,8 @@
           <t>testModels/db/11/m1101/m1101.off</t>
         </is>
       </c>
-      <c r="I39" t="inlineStr">
-        <is>
-          <t>[0.12567 0.57442 0.04093]</t>
-        </is>
+      <c r="I39" t="n">
+        <v>0.5894297571576562</v>
       </c>
       <c r="J39" t="n">
         <v>0.00567314313805</v>
@@ -2191,10 +2115,8 @@
           <t>testModels/db/11/m1102/m1102.off</t>
         </is>
       </c>
-      <c r="I40" t="inlineStr">
-        <is>
-          <t>[0.11303 0.6575  0.03694]</t>
-        </is>
+      <c r="I40" t="n">
+        <v>0.6681650375107182</v>
       </c>
       <c r="J40" t="n">
         <v>0.005296771457279999</v>
@@ -2235,10 +2157,8 @@
           <t>testModels/db/11/m1103/m1103.off</t>
         </is>
       </c>
-      <c r="I41" t="inlineStr">
-        <is>
-          <t>[0.11172 0.69397 0.05637]</t>
-        </is>
+      <c r="I41" t="n">
+        <v>0.7051657940854634</v>
       </c>
       <c r="J41" t="n">
         <v>0.007662401278960001</v>
@@ -2279,10 +2199,8 @@
           <t>testModels/db/11/m1104/m1104.off</t>
         </is>
       </c>
-      <c r="I42" t="inlineStr">
-        <is>
-          <t>[0.15579 0.52193 0.04802]</t>
-        </is>
+      <c r="I42" t="n">
+        <v>0.5468003297544165</v>
       </c>
       <c r="J42" t="n">
         <v>0.01177359342705</v>
@@ -2323,10 +2241,8 @@
           <t>testModels/db/11/m1105/m1105.off</t>
         </is>
       </c>
-      <c r="I43" t="inlineStr">
-        <is>
-          <t>[0.61554 0.18221 0.06342]</t>
-        </is>
+      <c r="I43" t="n">
+        <v>0.6450712313608011</v>
       </c>
       <c r="J43" t="n">
         <v>0.0176481641208</v>
@@ -2367,10 +2283,8 @@
           <t>testModels/db/11/m1106/m1106.off</t>
         </is>
       </c>
-      <c r="I44" t="inlineStr">
-        <is>
-          <t>[0.40875 0.16021 0.05349]</t>
-        </is>
+      <c r="I44" t="n">
+        <v>0.4422728383787655</v>
       </c>
       <c r="J44" t="n">
         <v>0.014774983832475</v>
@@ -2411,10 +2325,8 @@
           <t>testModels/db/11/m1107/m1107.off</t>
         </is>
       </c>
-      <c r="I45" t="inlineStr">
-        <is>
-          <t>[ 0.26337 -0.12316  0.4174 ]</t>
-        </is>
+      <c r="I45" t="n">
+        <v>0.5086847653847676</v>
       </c>
       <c r="J45" t="n">
         <v>0.0201794797352</v>
@@ -2455,10 +2367,8 @@
           <t>testModels/db/11/m1108/m1108.off</t>
         </is>
       </c>
-      <c r="I46" t="inlineStr">
-        <is>
-          <t>[ 0.70123 -2.56917  0.07835]</t>
-        </is>
+      <c r="I46" t="n">
+        <v>2.66430241025552</v>
       </c>
       <c r="J46" t="n">
         <v>0.03613536741282</v>
@@ -2499,10 +2409,8 @@
           <t>testModels/db/11/m1109/m1109.off</t>
         </is>
       </c>
-      <c r="I47" t="inlineStr">
-        <is>
-          <t>[ -0.74986 555.48224  -8.04175]</t>
-        </is>
+      <c r="I47" t="n">
+        <v>555.5409493419526</v>
       </c>
       <c r="J47" t="n">
         <v>0.07049502607000001</v>
@@ -2543,10 +2451,8 @@
           <t>testModels/db/11/m1110/m1110.off</t>
         </is>
       </c>
-      <c r="I48" t="inlineStr">
-        <is>
-          <t>[0.0859  0.47746 0.21317]</t>
-        </is>
+      <c r="I48" t="n">
+        <v>0.5298898577961842</v>
       </c>
       <c r="J48" t="n">
         <v>0.04253667849274999</v>
@@ -2587,10 +2493,8 @@
           <t>testModels/db/11/m1111/m1111.off</t>
         </is>
       </c>
-      <c r="I49" t="inlineStr">
-        <is>
-          <t>[0.18684 0.55625 0.08871]</t>
-        </is>
+      <c r="I49" t="n">
+        <v>0.5934552605671437</v>
       </c>
       <c r="J49" t="n">
         <v>0.0555498363525</v>
@@ -2631,10 +2535,8 @@
           <t>testModels/db/11/m1112/m1112.off</t>
         </is>
       </c>
-      <c r="I50" t="inlineStr">
-        <is>
-          <t>[-0.07558 -3.47315 -0.10452]</t>
-        </is>
+      <c r="I50" t="n">
+        <v>3.475545362880868</v>
       </c>
       <c r="J50" t="n">
         <v>0.03610291686859999</v>
@@ -2675,10 +2577,8 @@
           <t>testModels/db/12/m1200/m1200.off</t>
         </is>
       </c>
-      <c r="I51" t="inlineStr">
-        <is>
-          <t>[0.25469 0.07518 0.49447]</t>
-        </is>
+      <c r="I51" t="n">
+        <v>0.5612599461755092</v>
       </c>
       <c r="J51" t="n">
         <v>0.12001996886445</v>
@@ -2719,10 +2619,8 @@
           <t>testModels/db/12/m1201/m1201.off</t>
         </is>
       </c>
-      <c r="I52" t="inlineStr">
-        <is>
-          <t>[ 0.34536 -0.08818 -0.03426]</t>
-        </is>
+      <c r="I52" t="n">
+        <v>0.3580824644805655</v>
       </c>
       <c r="J52" t="n">
         <v>0.1842149637729</v>
@@ -2763,10 +2661,8 @@
           <t>testModels/db/12/m1202/m1202.off</t>
         </is>
       </c>
-      <c r="I53" t="inlineStr">
-        <is>
-          <t>[0.29561 0.07745 0.45725]</t>
-        </is>
+      <c r="I53" t="n">
+        <v>0.5499636795036806</v>
       </c>
       <c r="J53" t="n">
         <v>0.1072671295525</v>
@@ -2807,10 +2703,8 @@
           <t>testModels/db/12/m1203/m1203.off</t>
         </is>
       </c>
-      <c r="I54" t="inlineStr">
-        <is>
-          <t>[0.25843 0.56094 0.11652]</t>
-        </is>
+      <c r="I54" t="n">
+        <v>0.6285065483059072</v>
       </c>
       <c r="J54" t="n">
         <v>0.11261987743</v>
@@ -2851,10 +2745,8 @@
           <t>testModels/db/12/m1204/m1204.off</t>
         </is>
       </c>
-      <c r="I55" t="inlineStr">
-        <is>
-          <t>[0.34597 0.11028 0.55178]</t>
-        </is>
+      <c r="I55" t="n">
+        <v>0.6605424659875109</v>
       </c>
       <c r="J55" t="n">
         <v>0.1879373359802</v>
@@ -2895,10 +2787,8 @@
           <t>testModels/db/12/m1205/m1205.off</t>
         </is>
       </c>
-      <c r="I56" t="inlineStr">
-        <is>
-          <t>[0.48671 2.71782 0.19551]</t>
-        </is>
+      <c r="I56" t="n">
+        <v>2.767969582236098</v>
       </c>
       <c r="J56" t="n">
         <v>0.1366358164875</v>
@@ -2939,10 +2829,8 @@
           <t>testModels/db/12/m1206/m1206.off</t>
         </is>
       </c>
-      <c r="I57" t="inlineStr">
-        <is>
-          <t>[0.43004 0.07646 0.36512]</t>
-        </is>
+      <c r="I57" t="n">
+        <v>0.5692872062278712</v>
       </c>
       <c r="J57" t="n">
         <v>0.1560866223667202</v>
@@ -2983,10 +2871,8 @@
           <t>testModels/db/12/m1207/m1207.off</t>
         </is>
       </c>
-      <c r="I58" t="inlineStr">
-        <is>
-          <t>[0.71366 0.07172 0.32764]</t>
-        </is>
+      <c r="I58" t="n">
+        <v>0.7885412833955276</v>
       </c>
       <c r="J58" t="n">
         <v>0.04203211683450001</v>
@@ -3027,10 +2913,8 @@
           <t>testModels/db/12/m1208/m1208.off</t>
         </is>
       </c>
-      <c r="I59" t="inlineStr">
-        <is>
-          <t>[0.34902 0.1261  0.76561]</t>
-        </is>
+      <c r="I59" t="n">
+        <v>0.8508020822459635</v>
       </c>
       <c r="J59" t="n">
         <v>0.12773090537</v>
@@ -3071,10 +2955,8 @@
           <t>testModels/db/12/m1209/m1209.off</t>
         </is>
       </c>
-      <c r="I60" t="inlineStr">
-        <is>
-          <t>[0.50031 0.09729 0.49809]</t>
-        </is>
+      <c r="I60" t="n">
+        <v>0.7126481134184162</v>
       </c>
       <c r="J60" t="n">
         <v>0.216677963555</v>
@@ -3115,10 +2997,8 @@
           <t>testModels/db/12/m1210/m1210.off</t>
         </is>
       </c>
-      <c r="I61" t="inlineStr">
-        <is>
-          <t>[0.19287 0.02987 0.06621]</t>
-        </is>
+      <c r="I61" t="n">
+        <v>0.206089011229017</v>
       </c>
       <c r="J61" t="n">
         <v>0.124648111575</v>
@@ -3159,10 +3039,8 @@
           <t>testModels/db/12/m1211/m1211.off</t>
         </is>
       </c>
-      <c r="I62" t="inlineStr">
-        <is>
-          <t>[ 0.62244  0.43605 -2.70756]</t>
-        </is>
+      <c r="I62" t="n">
+        <v>2.812198903068106</v>
       </c>
       <c r="J62" t="n">
         <v>0.2484029286024999</v>
@@ -3203,10 +3081,8 @@
           <t>testModels/db/12/m1212/m1212.off</t>
         </is>
       </c>
-      <c r="I63" t="inlineStr">
-        <is>
-          <t>[0.56637 0.27271 1.91719]</t>
-        </is>
+      <c r="I63" t="n">
+        <v>2.017612802001679</v>
       </c>
       <c r="J63" t="n">
         <v>0.1672867212288</v>
@@ -3247,10 +3123,8 @@
           <t>testModels/db/13/m1300/m1300.off</t>
         </is>
       </c>
-      <c r="I64" t="inlineStr">
-        <is>
-          <t>[0.37423 0.03826 0.45334]</t>
-        </is>
+      <c r="I64" t="n">
+        <v>0.5890943699485118</v>
       </c>
       <c r="J64" t="n">
         <v>0.09872842770584998</v>
@@ -3291,10 +3165,8 @@
           <t>testModels/db/13/m1301/m1301.off</t>
         </is>
       </c>
-      <c r="I65" t="inlineStr">
-        <is>
-          <t>[0.33701 0.06132 0.43703]</t>
-        </is>
+      <c r="I65" t="n">
+        <v>0.5552752156943827</v>
       </c>
       <c r="J65" t="n">
         <v>0.066256415535</v>
@@ -3335,10 +3207,8 @@
           <t>testModels/db/13/m1302/m1302.off</t>
         </is>
       </c>
-      <c r="I66" t="inlineStr">
-        <is>
-          <t>[0.09855 0.11776 0.29435]</t>
-        </is>
+      <c r="I66" t="n">
+        <v>0.3319983216080078</v>
       </c>
       <c r="J66" t="n">
         <v>0.0470046237255</v>
@@ -3379,10 +3249,8 @@
           <t>testModels/db/13/m1303/m1303.off</t>
         </is>
       </c>
-      <c r="I67" t="inlineStr">
-        <is>
-          <t>[ 0.53583 -0.95418  0.22636]</t>
-        </is>
+      <c r="I67" t="n">
+        <v>1.117499070233687</v>
       </c>
       <c r="J67" t="n">
         <v>0.1985021710586999</v>
@@ -3423,10 +3291,8 @@
           <t>testModels/db/13/m1304/m1304.off</t>
         </is>
       </c>
-      <c r="I68" t="inlineStr">
-        <is>
-          <t>[0.1422  0.19537 0.59318]</t>
-        </is>
+      <c r="I68" t="n">
+        <v>0.6405115886122699</v>
       </c>
       <c r="J68" t="n">
         <v>0.07990405931970002</v>
@@ -3467,10 +3333,8 @@
           <t>testModels/db/13/m1305/m1305.off</t>
         </is>
       </c>
-      <c r="I69" t="inlineStr">
-        <is>
-          <t>[0.60234 0.1217  0.09605]</t>
-        </is>
+      <c r="I69" t="n">
+        <v>0.6219743019925619</v>
       </c>
       <c r="J69" t="n">
         <v>0.0331246069806</v>
@@ -3511,10 +3375,8 @@
           <t>testModels/db/13/m1306/m1306.off</t>
         </is>
       </c>
-      <c r="I70" t="inlineStr">
-        <is>
-          <t>[0.39563 0.15965 1.57998]</t>
-        </is>
+      <c r="I70" t="n">
+        <v>1.636563159574256</v>
       </c>
       <c r="J70" t="n">
         <v>0.1974030053342999</v>
@@ -3555,10 +3417,8 @@
           <t>testModels/db/13/m1307/m1307.off</t>
         </is>
       </c>
-      <c r="I71" t="inlineStr">
-        <is>
-          <t>[0.37587 0.14934 0.76889]</t>
-        </is>
+      <c r="I71" t="n">
+        <v>0.8687734293818027</v>
       </c>
       <c r="J71" t="n">
         <v>0.2160193265505</v>
@@ -3599,10 +3459,8 @@
           <t>testModels/db/13/m1308/m1308.off</t>
         </is>
       </c>
-      <c r="I72" t="inlineStr">
-        <is>
-          <t>[0.43055 0.11464 0.45177]</t>
-        </is>
+      <c r="I72" t="n">
+        <v>0.6345127315821533</v>
       </c>
       <c r="J72" t="n">
         <v>0.19138752451875</v>
@@ -3643,10 +3501,8 @@
           <t>testModels/db/13/m1309/m1309.off</t>
         </is>
       </c>
-      <c r="I73" t="inlineStr">
-        <is>
-          <t>[ 0.41695 -0.02927  0.11915]</t>
-        </is>
+      <c r="I73" t="n">
+        <v>0.4346234580226721</v>
       </c>
       <c r="J73" t="n">
         <v>0.14159001367225</v>
@@ -3687,10 +3543,8 @@
           <t>testModels/db/13/m1310/m1310.off</t>
         </is>
       </c>
-      <c r="I74" t="inlineStr">
-        <is>
-          <t>[0.40898 0.11903 0.60155]</t>
-        </is>
+      <c r="I74" t="n">
+        <v>0.7370804741394653</v>
       </c>
       <c r="J74" t="n">
         <v>0.1952923078799999</v>
@@ -3731,10 +3585,8 @@
           <t>testModels/db/13/m1311/m1311.off</t>
         </is>
       </c>
-      <c r="I75" t="inlineStr">
-        <is>
-          <t>[0.44071 0.09476 0.51214]</t>
-        </is>
+      <c r="I75" t="n">
+        <v>0.6822714190403661</v>
       </c>
       <c r="J75" t="n">
         <v>0.1431480521615</v>
@@ -3775,10 +3627,8 @@
           <t>testModels/db/13/m1312/m1312.off</t>
         </is>
       </c>
-      <c r="I76" t="inlineStr">
-        <is>
-          <t>[0.5001  0.17761 0.27906]</t>
-        </is>
+      <c r="I76" t="n">
+        <v>0.5996034562190253</v>
       </c>
       <c r="J76" t="n">
         <v>0.2215414359629999</v>
@@ -3819,10 +3669,8 @@
           <t>testModels/db/14/m1400/m1400.off</t>
         </is>
       </c>
-      <c r="I77" t="inlineStr">
-        <is>
-          <t>[0.32759 1.11689 0.11637]</t>
-        </is>
+      <c r="I77" t="n">
+        <v>1.16974626638147</v>
       </c>
       <c r="J77" t="n">
         <v>0.2061737382922</v>
@@ -3863,10 +3711,8 @@
           <t>testModels/db/14/m1401/m1401.off</t>
         </is>
       </c>
-      <c r="I78" t="inlineStr">
-        <is>
-          <t>[0.39782 0.37775 0.33055]</t>
-        </is>
+      <c r="I78" t="n">
+        <v>0.6404811368568801</v>
       </c>
       <c r="J78" t="n">
         <v>0.585685399061</v>
@@ -3907,10 +3753,8 @@
           <t>testModels/db/14/m1402/m1402.off</t>
         </is>
       </c>
-      <c r="I79" t="inlineStr">
-        <is>
-          <t>[ 0.16796 -1.03949 -3.40541]</t>
-        </is>
+      <c r="I79" t="n">
+        <v>3.564486434977824</v>
       </c>
       <c r="J79" t="n">
         <v>0.5856046431026</v>
@@ -3951,10 +3795,8 @@
           <t>testModels/db/14/m1403/m1403.off</t>
         </is>
       </c>
-      <c r="I80" t="inlineStr">
-        <is>
-          <t>[ 0.5     -0.19756 -0.61883]</t>
-        </is>
+      <c r="I80" t="n">
+        <v>0.819742337942043</v>
       </c>
       <c r="J80" t="n">
         <v>0.4645027603037999</v>
@@ -3995,10 +3837,8 @@
           <t>testModels/db/14/m1404/m1404.off</t>
         </is>
       </c>
-      <c r="I81" t="inlineStr">
-        <is>
-          <t>[0.3211  0.23671 0.52407]</t>
-        </is>
+      <c r="I81" t="n">
+        <v>0.6586212464423078</v>
       </c>
       <c r="J81" t="n">
         <v>0.2329240077266</v>
@@ -4039,10 +3879,8 @@
           <t>testModels/db/14/m1405/m1405.off</t>
         </is>
       </c>
-      <c r="I82" t="inlineStr">
-        <is>
-          <t>[ 0.3599  -0.03094 -0.00716]</t>
-        </is>
+      <c r="I82" t="n">
+        <v>0.3613023257726861</v>
       </c>
       <c r="J82" t="n">
         <v>0.5865306699874999</v>
@@ -4083,10 +3921,8 @@
           <t>testModels/db/14/m1406/m1406.off</t>
         </is>
       </c>
-      <c r="I83" t="inlineStr">
-        <is>
-          <t>[-0.66915 -0.02081 -0.54613]</t>
-        </is>
+      <c r="I83" t="n">
+        <v>0.8639761027006455</v>
       </c>
       <c r="J83" t="n">
         <v>0.0841694023968</v>
@@ -4127,10 +3963,8 @@
           <t>testModels/db/14/m1407/m1407.off</t>
         </is>
       </c>
-      <c r="I84" t="inlineStr">
-        <is>
-          <t>[0.4194  0.712   0.14076]</t>
-        </is>
+      <c r="I84" t="n">
+        <v>0.8382463080197116</v>
       </c>
       <c r="J84" t="n">
         <v>0.17019194710475</v>
@@ -4171,10 +4005,8 @@
           <t>testModels/db/14/m1408/m1408.off</t>
         </is>
       </c>
-      <c r="I85" t="inlineStr">
-        <is>
-          <t>[0.42832 0.17937 0.30331]</t>
-        </is>
+      <c r="I85" t="n">
+        <v>0.5546446857438891</v>
       </c>
       <c r="J85" t="n">
         <v>0.24976478682495</v>
@@ -4215,10 +4047,8 @@
           <t>testModels/db/14/m1409/m1409.off</t>
         </is>
       </c>
-      <c r="I86" t="inlineStr">
-        <is>
-          <t>[-0.07785  0.8428   0.97021]</t>
-        </is>
+      <c r="I86" t="n">
+        <v>1.287513252233688</v>
       </c>
       <c r="J86" t="n">
         <v>0.1642592688858</v>
@@ -4259,10 +4089,8 @@
           <t>testModels/db/14/m1410/m1410.off</t>
         </is>
       </c>
-      <c r="I87" t="inlineStr">
-        <is>
-          <t>[-0.36698 -1.20374 -0.41057]</t>
-        </is>
+      <c r="I87" t="n">
+        <v>1.323723885002757</v>
       </c>
       <c r="J87" t="n">
         <v>0.1278829525601129</v>
@@ -4303,10 +4131,8 @@
           <t>testModels/db/14/m1411/m1411.off</t>
         </is>
       </c>
-      <c r="I88" t="inlineStr">
-        <is>
-          <t>[0.60142 0.16156 0.15921]</t>
-        </is>
+      <c r="I88" t="n">
+        <v>0.642768959615704</v>
       </c>
       <c r="J88" t="n">
         <v>0.0939039850931</v>
@@ -4347,10 +4173,8 @@
           <t>testModels/db/14/m1412/m1412.off</t>
         </is>
       </c>
-      <c r="I89" t="inlineStr">
-        <is>
-          <t>[0.68541 0.21149 0.29044]</t>
-        </is>
+      <c r="I89" t="n">
+        <v>0.7738656385434007</v>
       </c>
       <c r="J89" t="n">
         <v>0.08440098270834998</v>
@@ -4391,10 +4215,8 @@
           <t>testModels/db/15/m1500/m1500.off</t>
         </is>
       </c>
-      <c r="I90" t="inlineStr">
-        <is>
-          <t>[0.22643 0.1993  0.58139]</t>
-        </is>
+      <c r="I90" t="n">
+        <v>0.6549786956999486</v>
       </c>
       <c r="J90" t="n">
         <v>0.1361507547867</v>
@@ -4435,10 +4257,8 @@
           <t>testModels/db/15/m1501/m1501.off</t>
         </is>
       </c>
-      <c r="I91" t="inlineStr">
-        <is>
-          <t>[0.27773 0.2798  0.62893]</t>
-        </is>
+      <c r="I91" t="n">
+        <v>0.7422720498921764</v>
       </c>
       <c r="J91" t="n">
         <v>0.19576849474065</v>
@@ -4479,10 +4299,8 @@
           <t>testModels/db/15/m1502/m1502.off</t>
         </is>
       </c>
-      <c r="I92" t="inlineStr">
-        <is>
-          <t>[0.42365 0.04181 0.16016]</t>
-        </is>
+      <c r="I92" t="n">
+        <v>0.4548392093646955</v>
       </c>
       <c r="J92" t="n">
         <v>0.0826927006095</v>
@@ -4523,10 +4341,8 @@
           <t>testModels/db/15/m1503/m1503.off</t>
         </is>
       </c>
-      <c r="I93" t="inlineStr">
-        <is>
-          <t>[0.34284 0.09837 0.12809]</t>
-        </is>
+      <c r="I93" t="n">
+        <v>0.3789775151125117</v>
       </c>
       <c r="J93" t="n">
         <v>0.03216136113819999</v>
@@ -4567,10 +4383,8 @@
           <t>testModels/db/15/m1504/m1504.off</t>
         </is>
       </c>
-      <c r="I94" t="inlineStr">
-        <is>
-          <t>[0.23779 0.05134 0.48981]</t>
-        </is>
+      <c r="I94" t="n">
+        <v>0.5468981341886293</v>
       </c>
       <c r="J94" t="n">
         <v>0.0758695732669</v>
@@ -4611,10 +4425,8 @@
           <t>testModels/db/15/m1505/m1505.off</t>
         </is>
       </c>
-      <c r="I95" t="inlineStr">
-        <is>
-          <t>[0.20814 0.07373 0.40945]</t>
-        </is>
+      <c r="I95" t="n">
+        <v>0.4651962912917554</v>
       </c>
       <c r="J95" t="n">
         <v>0.0645418395294</v>
@@ -4655,10 +4467,8 @@
           <t>testModels/db/15/m1506/m1506.off</t>
         </is>
       </c>
-      <c r="I96" t="inlineStr">
-        <is>
-          <t>[0.34827 1.43765 0.49832]</t>
-        </is>
+      <c r="I96" t="n">
+        <v>1.560915220978554</v>
       </c>
       <c r="J96" t="n">
         <v>0.1288943364284</v>
@@ -4699,10 +4509,8 @@
           <t>testModels/db/15/m1507/m1507.off</t>
         </is>
       </c>
-      <c r="I97" t="inlineStr">
-        <is>
-          <t>[0.23162 0.08924 0.45453]</t>
-        </is>
+      <c r="I97" t="n">
+        <v>0.5178890063493991</v>
       </c>
       <c r="J97" t="n">
         <v>0.07374694566604999</v>
@@ -4743,10 +4551,8 @@
           <t>testModels/db/15/m1508/m1508.off</t>
         </is>
       </c>
-      <c r="I98" t="inlineStr">
-        <is>
-          <t>[0.49715 0.04413 0.31961]</t>
-        </is>
+      <c r="I98" t="n">
+        <v>0.5926709516310176</v>
       </c>
       <c r="J98" t="n">
         <v>0.07039702126274998</v>
@@ -4787,10 +4593,8 @@
           <t>testModels/db/15/m1509/m1509.off</t>
         </is>
       </c>
-      <c r="I99" t="inlineStr">
-        <is>
-          <t>[0.29106 0.16618 0.54691]</t>
-        </is>
+      <c r="I99" t="n">
+        <v>0.6414435012033664</v>
       </c>
       <c r="J99" t="n">
         <v>0.1811462751618</v>
@@ -4831,10 +4635,8 @@
           <t>testModels/db/15/m1510/m1510.off</t>
         </is>
       </c>
-      <c r="I100" t="inlineStr">
-        <is>
-          <t>[0.25768 0.09251 0.46593]</t>
-        </is>
+      <c r="I100" t="n">
+        <v>0.5404144798045344</v>
       </c>
       <c r="J100" t="n">
         <v>0.09692012567019999</v>
@@ -4875,10 +4677,8 @@
           <t>testModels/db/15/m1511/m1511.off</t>
         </is>
       </c>
-      <c r="I101" t="inlineStr">
-        <is>
-          <t>[0.30445 0.08735 0.59198]</t>
-        </is>
+      <c r="I101" t="n">
+        <v>0.6713896582725891</v>
       </c>
       <c r="J101" t="n">
         <v>0.119308459153</v>
@@ -4919,10 +4719,8 @@
           <t>testModels/db/15/m1512/m1512.off</t>
         </is>
       </c>
-      <c r="I102" t="inlineStr">
-        <is>
-          <t>[0.53662 0.16367 0.1268 ]</t>
-        </is>
+      <c r="I102" t="n">
+        <v>0.5751799931608572</v>
       </c>
       <c r="J102" t="n">
         <v>0.07504459125004999</v>
@@ -4963,10 +4761,8 @@
           <t>testModels/db/16/m1600/m1600.off</t>
         </is>
       </c>
-      <c r="I103" t="inlineStr">
-        <is>
-          <t>[0.23492 0.36545 0.23473]</t>
-        </is>
+      <c r="I103" t="n">
+        <v>0.4938009535455633</v>
       </c>
       <c r="J103" t="n">
         <v>0.16730878970505</v>
@@ -5007,10 +4803,8 @@
           <t>testModels/db/16/m1601/m1601.off</t>
         </is>
       </c>
-      <c r="I104" t="inlineStr">
-        <is>
-          <t>[0.29056 0.30705 0.29047]</t>
-        </is>
+      <c r="I104" t="n">
+        <v>0.5129148151804925</v>
       </c>
       <c r="J104" t="n">
         <v>0.267326072757</v>
@@ -5051,10 +4845,8 @@
           <t>testModels/db/16/m1602/m1602.off</t>
         </is>
       </c>
-      <c r="I105" t="inlineStr">
-        <is>
-          <t>[ 0.21517 10.64896  0.21541]</t>
-        </is>
+      <c r="I105" t="n">
+        <v>10.65330892710382</v>
       </c>
       <c r="J105" t="n">
         <v>0.1372117698392</v>
@@ -5095,10 +4887,8 @@
           <t>testModels/db/16/m1603/m1603.off</t>
         </is>
       </c>
-      <c r="I106" t="inlineStr">
-        <is>
-          <t>[0.20474 0.37498 0.20439]</t>
-        </is>
+      <c r="I106" t="n">
+        <v>0.4736077918143534</v>
       </c>
       <c r="J106" t="n">
         <v>0.12268194633695</v>
@@ -5139,10 +4929,8 @@
           <t>testModels/db/16/m1604/m1604.off</t>
         </is>
       </c>
-      <c r="I107" t="inlineStr">
-        <is>
-          <t>[0.2197  0.36789 0.22455]</t>
-        </is>
+      <c r="I107" t="n">
+        <v>0.4837704005043448</v>
       </c>
       <c r="J107" t="n">
         <v>0.14381334482895</v>
@@ -5183,10 +4971,8 @@
           <t>testModels/db/16/m1605/m1605.off</t>
         </is>
       </c>
-      <c r="I108" t="inlineStr">
-        <is>
-          <t>[0.34164 0.32351 0.35603]</t>
-        </is>
+      <c r="I108" t="n">
+        <v>0.5900303134020558</v>
       </c>
       <c r="J108" t="n">
         <v>0.3810551544445499</v>
@@ -5227,10 +5013,8 @@
           <t>testModels/db/16/m1606/m1606.off</t>
         </is>
       </c>
-      <c r="I109" t="inlineStr">
-        <is>
-          <t>[0.34754 0.32821 0.32604]</t>
-        </is>
+      <c r="I109" t="n">
+        <v>0.5786225054700455</v>
       </c>
       <c r="J109" t="n">
         <v>0.3432074538341999</v>
@@ -5271,10 +5055,8 @@
           <t>testModels/db/16/m1607/m1607.off</t>
         </is>
       </c>
-      <c r="I110" t="inlineStr">
-        <is>
-          <t>[0.27381 9.61377 0.27599]</t>
-        </is>
+      <c r="I110" t="n">
+        <v>9.621629683250177</v>
       </c>
       <c r="J110" t="n">
         <v>0.2316390123008</v>
@@ -5315,10 +5097,8 @@
           <t>testModels/db/16/m1608/m1608.off</t>
         </is>
       </c>
-      <c r="I111" t="inlineStr">
-        <is>
-          <t>[0.425   0.44919 0.425  ]</t>
-        </is>
+      <c r="I111" t="n">
+        <v>0.7503495583547535</v>
       </c>
       <c r="J111" t="n">
         <v>0.6079999999999999</v>
@@ -5359,10 +5139,8 @@
           <t>testModels/db/16/m1609/m1609.off</t>
         </is>
       </c>
-      <c r="I112" t="inlineStr">
-        <is>
-          <t>[0.27568 0.35811 0.27568]</t>
-        </is>
+      <c r="I112" t="n">
+        <v>0.5293811403815504</v>
       </c>
       <c r="J112" t="n">
         <v>0.23880042525455</v>
@@ -5403,10 +5181,8 @@
           <t>testModels/db/16/m1610/m1610.off</t>
         </is>
       </c>
-      <c r="I113" t="inlineStr">
-        <is>
-          <t>[0.33557 0.35663 0.33541]</t>
-        </is>
+      <c r="I113" t="n">
+        <v>0.5935444082093195</v>
       </c>
       <c r="J113" t="n">
         <v>0.3663335584208999</v>
@@ -5447,10 +5223,8 @@
           <t>testModels/db/16/m1611/m1611.off</t>
         </is>
       </c>
-      <c r="I114" t="inlineStr">
-        <is>
-          <t>[0.61155 0.26853 0.26853]</t>
-        </is>
+      <c r="I114" t="n">
+        <v>0.7198678966021049</v>
       </c>
       <c r="J114" t="n">
         <v>0.22536144437375</v>
@@ -5491,10 +5265,8 @@
           <t>testModels/db/16/m1612/m1612.off</t>
         </is>
       </c>
-      <c r="I115" t="inlineStr">
-        <is>
-          <t>[0.22461 4.34884 0.22458]</t>
-        </is>
+      <c r="I115" t="n">
+        <v>4.360426081208259</v>
       </c>
       <c r="J115" t="n">
         <v>0.1513558239525</v>
@@ -5535,10 +5307,8 @@
           <t>testModels/db/17/m1700/m1700.off</t>
         </is>
       </c>
-      <c r="I116" t="inlineStr">
-        <is>
-          <t>[ 0.50313 -0.06476  0.3562 ]</t>
-        </is>
+      <c r="I116" t="n">
+        <v>0.6198455781716755</v>
       </c>
       <c r="J116" t="n">
         <v>0.38632799271675</v>
@@ -5579,10 +5349,8 @@
           <t>testModels/db/17/m1701/m1701.off</t>
         </is>
       </c>
-      <c r="I117" t="inlineStr">
-        <is>
-          <t>[0.5     0.55113 0.26898]</t>
-        </is>
+      <c r="I117" t="n">
+        <v>0.7912623713546214</v>
       </c>
       <c r="J117" t="n">
         <v>0.2997184795742999</v>
@@ -5623,10 +5391,8 @@
           <t>testModels/db/17/m1702/m1702.off</t>
         </is>
       </c>
-      <c r="I118" t="inlineStr">
-        <is>
-          <t>[0.5     0.31679 0.26274]</t>
-        </is>
+      <c r="I118" t="n">
+        <v>0.6476045935389062</v>
       </c>
       <c r="J118" t="n">
         <v>0.2787690292414</v>
@@ -5667,10 +5433,8 @@
           <t>testModels/db/17/m1703/m1703.off</t>
         </is>
       </c>
-      <c r="I119" t="inlineStr">
-        <is>
-          <t>[0.35418 0.41692 0.50967]</t>
-        </is>
+      <c r="I119" t="n">
+        <v>0.74768074137693</v>
       </c>
       <c r="J119" t="n">
         <v>0.6194081680999999</v>
@@ -5711,10 +5475,8 @@
           <t>testModels/db/17/m1704/m1704.off</t>
         </is>
       </c>
-      <c r="I120" t="inlineStr">
-        <is>
-          <t>[0.42804 0.33992 0.36365]</t>
-        </is>
+      <c r="I120" t="n">
+        <v>0.6565078561121291</v>
       </c>
       <c r="J120" t="n">
         <v>0.5461226671774999</v>
@@ -5755,10 +5517,8 @@
           <t>testModels/db/17/m1705/m1705.off</t>
         </is>
       </c>
-      <c r="I121" t="inlineStr">
-        <is>
-          <t>[0.29051 0.50058 0.0298 ]</t>
-        </is>
+      <c r="I121" t="n">
+        <v>0.5795370022426829</v>
       </c>
       <c r="J121" t="n">
         <v>0.02653413475437499</v>
@@ -5799,10 +5559,8 @@
           <t>testModels/db/17/m1706/m1706.off</t>
         </is>
       </c>
-      <c r="I122" t="inlineStr">
-        <is>
-          <t>[ 0.03585 -0.01421 -1.92436]</t>
-        </is>
+      <c r="I122" t="n">
+        <v>1.924747619700219</v>
       </c>
       <c r="J122" t="n">
         <v>0.014289598375</v>
@@ -5843,10 +5601,8 @@
           <t>testModels/db/17/m1707/m1707.off</t>
         </is>
       </c>
-      <c r="I123" t="inlineStr">
-        <is>
-          <t>[ 0.26842 -0.84978 -2.73226]</t>
-        </is>
+      <c r="I123" t="n">
+        <v>2.87391802916773</v>
       </c>
       <c r="J123" t="n">
         <v>0.12699258673075</v>
@@ -5887,10 +5643,8 @@
           <t>testModels/db/17/m1708/m1708.off</t>
         </is>
       </c>
-      <c r="I124" t="inlineStr">
-        <is>
-          <t>[0.27248 0.45843 0.12625]</t>
-        </is>
+      <c r="I124" t="n">
+        <v>0.5480399341627323</v>
       </c>
       <c r="J124" t="n">
         <v>0.01399797760203499</v>
@@ -5931,10 +5685,8 @@
           <t>testModels/db/17/m1709/m1709.off</t>
         </is>
       </c>
-      <c r="I125" t="inlineStr">
-        <is>
-          <t>[ 0.01618 -0.0001  -0.0161 ]</t>
-        </is>
+      <c r="I125" t="n">
+        <v>0.02282710625452686</v>
       </c>
       <c r="J125" t="n">
         <v>0.005889478087669998</v>
@@ -5975,10 +5727,8 @@
           <t>testModels/db/17/m1710/m1710.off</t>
         </is>
       </c>
-      <c r="I126" t="inlineStr">
-        <is>
-          <t>[0.28876 0.49429 0.07245]</t>
-        </is>
+      <c r="I126" t="n">
+        <v>0.5770248902467106</v>
       </c>
       <c r="J126" t="n">
         <v>0.0468769388463</v>
@@ -6019,10 +5769,8 @@
           <t>testModels/db/17/m1711/m1711.off</t>
         </is>
       </c>
-      <c r="I127" t="inlineStr">
-        <is>
-          <t>[0.17116 0.5154  0.07614]</t>
-        </is>
+      <c r="I127" t="n">
+        <v>0.5483873210121538</v>
       </c>
       <c r="J127" t="n">
         <v>0.022203345375</v>
@@ -6063,10 +5811,8 @@
           <t>testModels/db/17/m1712/m1712.off</t>
         </is>
       </c>
-      <c r="I128" t="inlineStr">
-        <is>
-          <t>[0.25076 0.50101 0.0566 ]</t>
-        </is>
+      <c r="I128" t="n">
+        <v>0.5631075208341388</v>
       </c>
       <c r="J128" t="n">
         <v>0.0275369728818</v>
@@ -6107,10 +5853,8 @@
           <t>testModels/db/18/m1800/m1800.off</t>
         </is>
       </c>
-      <c r="I129" t="inlineStr">
-        <is>
-          <t>[0.51523 0.31951 0.13599]</t>
-        </is>
+      <c r="I129" t="n">
+        <v>0.6213244117082173</v>
       </c>
       <c r="J129" t="n">
         <v>0.5039622732186</v>
@@ -6151,10 +5895,8 @@
           <t>testModels/db/18/m1801/m1801.off</t>
         </is>
       </c>
-      <c r="I130" t="inlineStr">
-        <is>
-          <t>[0.45024 0.95485 0.34228]</t>
-        </is>
+      <c r="I130" t="n">
+        <v>1.10978267848802</v>
       </c>
       <c r="J130" t="n">
         <v>0.5839181688284999</v>
@@ -6195,10 +5937,8 @@
           <t>testModels/db/18/m1802/m1802.off</t>
         </is>
       </c>
-      <c r="I131" t="inlineStr">
-        <is>
-          <t>[0.511   0.16634 0.19297]</t>
-        </is>
+      <c r="I131" t="n">
+        <v>0.5709874283546265</v>
       </c>
       <c r="J131" t="n">
         <v>0.3518480536242</v>
@@ -6239,10 +5979,8 @@
           <t>testModels/db/18/m1803/m1803.off</t>
         </is>
       </c>
-      <c r="I132" t="inlineStr">
-        <is>
-          <t>[0.36383 2.77827 1.81706]</t>
-        </is>
+      <c r="I132" t="n">
+        <v>3.339593683144616</v>
       </c>
       <c r="J132" t="n">
         <v>0.5595389763159</v>
@@ -6283,10 +6021,8 @@
           <t>testModels/db/18/m1804/m1804.off</t>
         </is>
       </c>
-      <c r="I133" t="inlineStr">
-        <is>
-          <t>[0.28563 0.43037 0.24735]</t>
-        </is>
+      <c r="I133" t="n">
+        <v>0.5727008617910611</v>
       </c>
       <c r="J133" t="n">
         <v>0.2981086693236</v>
@@ -6327,10 +6063,8 @@
           <t>testModels/db/18/m1805/m1805.off</t>
         </is>
       </c>
-      <c r="I134" t="inlineStr">
-        <is>
-          <t>[0.24185 0.04264 0.19024]</t>
-        </is>
+      <c r="I134" t="n">
+        <v>0.3106496813581565</v>
       </c>
       <c r="J134" t="n">
         <v>0.25429138871805</v>
@@ -6371,10 +6105,8 @@
           <t>testModels/db/18/m1806/m1806.off</t>
         </is>
       </c>
-      <c r="I135" t="inlineStr">
-        <is>
-          <t>[0.33564 0.45564 0.20624]</t>
-        </is>
+      <c r="I135" t="n">
+        <v>0.6023279965570014</v>
       </c>
       <c r="J135" t="n">
         <v>0.3667566974668</v>
@@ -6415,10 +6147,8 @@
           <t>testModels/db/18/m1807/m1807.off</t>
         </is>
       </c>
-      <c r="I136" t="inlineStr">
-        <is>
-          <t>[0.54541 0.12922 0.36112]</t>
-        </is>
+      <c r="I136" t="n">
+        <v>0.6667638443153735</v>
       </c>
       <c r="J136" t="n">
         <v>0.1942775707323</v>
@@ -6459,10 +6189,8 @@
           <t>testModels/db/18/m1808/m1808.off</t>
         </is>
       </c>
-      <c r="I137" t="inlineStr">
-        <is>
-          <t>[0.39233 0.41869 0.41794]</t>
-        </is>
+      <c r="I137" t="n">
+        <v>0.7098625048574279</v>
       </c>
       <c r="J137" t="n">
         <v>0.60615035958075</v>
@@ -6503,10 +6231,8 @@
           <t>testModels/db/18/m1809/m1809.off</t>
         </is>
       </c>
-      <c r="I138" t="inlineStr">
-        <is>
-          <t>[0.49982 0.16092 0.28351]</t>
-        </is>
+      <c r="I138" t="n">
+        <v>0.5967372119898237</v>
       </c>
       <c r="J138" t="n">
         <v>0.2841935748727499</v>
@@ -6547,10 +6273,8 @@
           <t>testModels/db/18/m1810/m1810.off</t>
         </is>
       </c>
-      <c r="I139" t="inlineStr">
-        <is>
-          <t>[ 0.50142 -0.20934  0.36146]</t>
-        </is>
+      <c r="I139" t="n">
+        <v>0.6526083143767877</v>
       </c>
       <c r="J139" t="n">
         <v>0.231584768836</v>
@@ -6591,10 +6315,8 @@
           <t>testModels/db/18/m1811/m1811.off</t>
         </is>
       </c>
-      <c r="I140" t="inlineStr">
-        <is>
-          <t>[0.42233 0.95945 1.03998]</t>
-        </is>
+      <c r="I140" t="n">
+        <v>1.476636120981594</v>
       </c>
       <c r="J140" t="n">
         <v>0.5604020983959999</v>
@@ -6635,10 +6357,8 @@
           <t>testModels/db/18/m1812/m1812.off</t>
         </is>
       </c>
-      <c r="I141" t="inlineStr">
-        <is>
-          <t>[ 0.28292  0.95459 -0.47501]</t>
-        </is>
+      <c r="I141" t="n">
+        <v>1.103140169297351</v>
       </c>
       <c r="J141" t="n">
         <v>0.09693337393699998</v>
@@ -6679,10 +6399,8 @@
           <t>testModels/db/18/m1813/m1813.off</t>
         </is>
       </c>
-      <c r="I142" t="inlineStr">
-        <is>
-          <t>[ 0.35783  0.15391 -0.69514]</t>
-        </is>
+      <c r="I142" t="n">
+        <v>0.7968329866019411</v>
       </c>
       <c r="J142" t="n">
         <v>0.55862034481525</v>
@@ -6723,10 +6441,8 @@
           <t>testModels/db/18/m1814/m1814.off</t>
         </is>
       </c>
-      <c r="I143" t="inlineStr">
-        <is>
-          <t>[0.22933 0.45598 0.52142]</t>
-        </is>
+      <c r="I143" t="n">
+        <v>0.7296480297390275</v>
       </c>
       <c r="J143" t="n">
         <v>0.7130584857292499</v>
@@ -6767,10 +6483,8 @@
           <t>testModels/db/2/m200/m200.off</t>
         </is>
       </c>
-      <c r="I144" t="inlineStr">
-        <is>
-          <t>[0.21667 0.17405 0.09835]</t>
-        </is>
+      <c r="I144" t="n">
+        <v>0.2948098828131037</v>
       </c>
       <c r="J144" t="n">
         <v>0.0629806609719</v>
@@ -6811,10 +6525,8 @@
           <t>testModels/db/2/m201/m201.off</t>
         </is>
       </c>
-      <c r="I145" t="inlineStr">
-        <is>
-          <t>[0.32969 0.13545 0.34994]</t>
-        </is>
+      <c r="I145" t="n">
+        <v>0.4995024295394319</v>
       </c>
       <c r="J145" t="n">
         <v>0.13366499845625</v>
@@ -6855,10 +6567,8 @@
           <t>testModels/db/2/m202/m202.off</t>
         </is>
       </c>
-      <c r="I146" t="inlineStr">
-        <is>
-          <t>[0.16031 0.53395 0.09177]</t>
-        </is>
+      <c r="I146" t="n">
+        <v>0.5650001280664023</v>
       </c>
       <c r="J146" t="n">
         <v>0.0516014193972</v>
@@ -6899,10 +6609,8 @@
           <t>testModels/db/2/m203/m203.off</t>
         </is>
       </c>
-      <c r="I147" t="inlineStr">
-        <is>
-          <t>[0.18661 0.41486 0.12281]</t>
-        </is>
+      <c r="I147" t="n">
+        <v>0.471185126747117</v>
       </c>
       <c r="J147" t="n">
         <v>0.06315912987</v>
@@ -6943,10 +6651,8 @@
           <t>testModels/db/2/m204/m204.off</t>
         </is>
       </c>
-      <c r="I148" t="inlineStr">
-        <is>
-          <t>[0.1833  0.51217 0.11139]</t>
-        </is>
+      <c r="I148" t="n">
+        <v>0.5552728333083351</v>
       </c>
       <c r="J148" t="n">
         <v>0.09861214600439998</v>
@@ -6987,10 +6693,8 @@
           <t>testModels/db/2/m205/m205.off</t>
         </is>
       </c>
-      <c r="I149" t="inlineStr">
-        <is>
-          <t>[0.20338 0.55405 0.116  ]</t>
-        </is>
+      <c r="I149" t="n">
+        <v>0.6014943298523155</v>
       </c>
       <c r="J149" t="n">
         <v>0.070458809638</v>
@@ -7031,10 +6735,8 @@
           <t>testModels/db/2/m206/m206.off</t>
         </is>
       </c>
-      <c r="I150" t="inlineStr">
-        <is>
-          <t>[0.16246 0.17742 0.76588]</t>
-        </is>
+      <c r="I150" t="n">
+        <v>0.8027768093249181</v>
       </c>
       <c r="J150" t="n">
         <v>0.0579511642269</v>
@@ -7075,10 +6777,8 @@
           <t>testModels/db/2/m207/m207.off</t>
         </is>
       </c>
-      <c r="I151" t="inlineStr">
-        <is>
-          <t>[0.20774 0.76449 0.09746]</t>
-        </is>
+      <c r="I151" t="n">
+        <v>0.7981822167103412</v>
       </c>
       <c r="J151" t="n">
         <v>0.08830113672149997</v>
@@ -7119,10 +6819,8 @@
           <t>testModels/db/2/m208/m208.off</t>
         </is>
       </c>
-      <c r="I152" t="inlineStr">
-        <is>
-          <t>[0.19666 0.57249 0.09086]</t>
-        </is>
+      <c r="I152" t="n">
+        <v>0.6121087592214904</v>
       </c>
       <c r="J152" t="n">
         <v>0.0502958286896</v>
@@ -7163,10 +6861,8 @@
           <t>testModels/db/2/m209/m209.off</t>
         </is>
       </c>
-      <c r="I153" t="inlineStr">
-        <is>
-          <t>[0.21522 0.65946 0.17456]</t>
-        </is>
+      <c r="I153" t="n">
+        <v>0.7153164380604121</v>
       </c>
       <c r="J153" t="n">
         <v>0.09699395964644997</v>
@@ -7207,10 +6903,8 @@
           <t>testModels/db/2/m210/m210.off</t>
         </is>
       </c>
-      <c r="I154" t="inlineStr">
-        <is>
-          <t>[0.30551 0.56034 0.18115]</t>
-        </is>
+      <c r="I154" t="n">
+        <v>0.6634231530029858</v>
       </c>
       <c r="J154" t="n">
         <v>0.3257943964477499</v>
@@ -7251,10 +6945,8 @@
           <t>testModels/db/2/m211/m211.off</t>
         </is>
       </c>
-      <c r="I155" t="inlineStr">
-        <is>
-          <t>[0.18333 0.54343 0.12006]</t>
-        </is>
+      <c r="I155" t="n">
+        <v>0.585953083725378</v>
       </c>
       <c r="J155" t="n">
         <v>0.06076322891144999</v>
@@ -7295,10 +6987,8 @@
           <t>testModels/db/2/m212/m212.off</t>
         </is>
       </c>
-      <c r="I156" t="inlineStr">
-        <is>
-          <t>[0.28705 0.52404 0.10317]</t>
-        </is>
+      <c r="I156" t="n">
+        <v>0.6063492839013889</v>
       </c>
       <c r="J156" t="n">
         <v>0.07985204410555001</v>
@@ -7339,10 +7029,8 @@
           <t>testModels/db/3/m300/m300.off</t>
         </is>
       </c>
-      <c r="I157" t="inlineStr">
-        <is>
-          <t>[0.33935 0.08242 1.22676]</t>
-        </is>
+      <c r="I157" t="n">
+        <v>1.275494816908894</v>
       </c>
       <c r="J157" t="n">
         <v>0.272133783058827</v>
@@ -7383,10 +7071,8 @@
           <t>testModels/db/3/m301/m301.off</t>
         </is>
       </c>
-      <c r="I158" t="inlineStr">
-        <is>
-          <t>[ 0.08329  0.09585 -0.75625]</t>
-        </is>
+      <c r="I158" t="n">
+        <v>0.7668358929631715</v>
       </c>
       <c r="J158" t="n">
         <v>0.42176198758065</v>
@@ -7427,10 +7113,8 @@
           <t>testModels/db/3/m302/m302.off</t>
         </is>
       </c>
-      <c r="I159" t="inlineStr">
-        <is>
-          <t>[0.40543 0.23625 0.50762]</t>
-        </is>
+      <c r="I159" t="n">
+        <v>0.6912807370527623</v>
       </c>
       <c r="J159" t="n">
         <v>0.44863801136315</v>
@@ -7471,10 +7155,8 @@
           <t>testModels/db/3/m303/m303.off</t>
         </is>
       </c>
-      <c r="I160" t="inlineStr">
-        <is>
-          <t>[ 0.34177 -0.05775  0.4675 ]</t>
-        </is>
+      <c r="I160" t="n">
+        <v>0.5819743024468653</v>
       </c>
       <c r="J160" t="n">
         <v>0.4799720971559999</v>
@@ -7515,10 +7197,8 @@
           <t>testModels/db/3/m304/m304.off</t>
         </is>
       </c>
-      <c r="I161" t="inlineStr">
-        <is>
-          <t>[ 0.44621 -0.21781  0.71867]</t>
-        </is>
+      <c r="I161" t="n">
+        <v>0.8735197457876698</v>
       </c>
       <c r="J161" t="n">
         <v>0.5246717629299</v>
@@ -7559,10 +7239,8 @@
           <t>testModels/db/3/m305/m305.off</t>
         </is>
       </c>
-      <c r="I162" t="inlineStr">
-        <is>
-          <t>[0.32742 0.55    0.17718]</t>
-        </is>
+      <c r="I162" t="n">
+        <v>0.6641498529799693</v>
       </c>
       <c r="J162" t="n">
         <v>0.2091357947613</v>
@@ -7603,10 +7281,8 @@
           <t>testModels/db/3/m306/m306.off</t>
         </is>
       </c>
-      <c r="I163" t="inlineStr">
-        <is>
-          <t>[0.38818 0.29526 0.76387]</t>
-        </is>
+      <c r="I163" t="n">
+        <v>0.9062922246344396</v>
       </c>
       <c r="J163" t="n">
         <v>0.5021063473894</v>
@@ -7647,10 +7323,8 @@
           <t>testModels/db/3/m307/m307.off</t>
         </is>
       </c>
-      <c r="I164" t="inlineStr">
-        <is>
-          <t>[0.32987 0.44546 0.18796]</t>
-        </is>
+      <c r="I164" t="n">
+        <v>0.5853048029009464</v>
       </c>
       <c r="J164" t="n">
         <v>0.2854492755504</v>
@@ -7691,10 +7365,8 @@
           <t>testModels/db/3/m308/m308.off</t>
         </is>
       </c>
-      <c r="I165" t="inlineStr">
-        <is>
-          <t>[ 0.23438 -0.11465 -0.01409]</t>
-        </is>
+      <c r="I165" t="n">
+        <v>0.2612976627589222</v>
       </c>
       <c r="J165" t="n">
         <v>0.1345423657043896</v>
@@ -7735,10 +7407,8 @@
           <t>testModels/db/3/m309/m309.off</t>
         </is>
       </c>
-      <c r="I166" t="inlineStr">
-        <is>
-          <t>[ 0.12636 -0.2492  -0.12181]</t>
-        </is>
+      <c r="I166" t="n">
+        <v>0.3047996693557312</v>
       </c>
       <c r="J166" t="n">
         <v>0.05283930541306872</v>
@@ -7779,10 +7449,8 @@
           <t>testModels/db/3/m310/m310.off</t>
         </is>
       </c>
-      <c r="I167" t="inlineStr">
-        <is>
-          <t>[ 0.28511 -0.00504 -0.03517]</t>
-        </is>
+      <c r="I167" t="n">
+        <v>0.2873133122593487</v>
       </c>
       <c r="J167" t="n">
         <v>0.1180692170551223</v>
@@ -7823,10 +7491,8 @@
           <t>testModels/db/3/m311/m311.off</t>
         </is>
       </c>
-      <c r="I168" t="inlineStr">
-        <is>
-          <t>[0.23408 0.07864 0.07801]</t>
-        </is>
+      <c r="I168" t="n">
+        <v>0.2589699424232592</v>
       </c>
       <c r="J168" t="n">
         <v>0.1477825613933806</v>
@@ -7867,10 +7533,8 @@
           <t>testModels/db/3/m312/m312.off</t>
         </is>
       </c>
-      <c r="I169" t="inlineStr">
-        <is>
-          <t>[ 0.26322  0.04064 -0.02771]</t>
-        </is>
+      <c r="I169" t="n">
+        <v>0.2677723957968401</v>
       </c>
       <c r="J169" t="n">
         <v>0.1353662284264502</v>
@@ -7911,10 +7575,8 @@
           <t>testModels/db/4/m400/m400.off</t>
         </is>
       </c>
-      <c r="I170" t="inlineStr">
-        <is>
-          <t>[0.40094 0.2333  0.48854]</t>
-        </is>
+      <c r="I170" t="n">
+        <v>0.6736874996811439</v>
       </c>
       <c r="J170" t="n">
         <v>0.5465683954868</v>
@@ -7955,10 +7617,8 @@
           <t>testModels/db/4/m401/m401.off</t>
         </is>
       </c>
-      <c r="I171" t="inlineStr">
-        <is>
-          <t>[0.53416 0.07716 0.65824]</t>
-        </is>
+      <c r="I171" t="n">
+        <v>0.8512148037298419</v>
       </c>
       <c r="J171" t="n">
         <v>0.163505925</v>
@@ -7999,10 +7659,8 @@
           <t>testModels/db/4/m402/m402.off</t>
         </is>
       </c>
-      <c r="I172" t="inlineStr">
-        <is>
-          <t>[0.32407 0.28076 0.33032]</t>
-        </is>
+      <c r="I172" t="n">
+        <v>0.5412540668923238</v>
       </c>
       <c r="J172" t="n">
         <v>0.3803311612695</v>
@@ -8043,10 +7701,8 @@
           <t>testModels/db/4/m403/m403.off</t>
         </is>
       </c>
-      <c r="I173" t="inlineStr">
-        <is>
-          <t>[0.49995 0.20469 0.49994]</t>
-        </is>
+      <c r="I173" t="n">
+        <v>0.7360560226147552</v>
       </c>
       <c r="J173" t="n">
         <v>0.4723955749999999</v>
@@ -8087,10 +7743,8 @@
           <t>testModels/db/4/m404/m404.off</t>
         </is>
       </c>
-      <c r="I174" t="inlineStr">
-        <is>
-          <t>[0.40153 0.13608 0.43336]</t>
-        </is>
+      <c r="I174" t="n">
+        <v>0.6062568140491283</v>
       </c>
       <c r="J174" t="n">
         <v>0.2758108135843</v>
@@ -8131,10 +7785,8 @@
           <t>testModels/db/4/m405/m405.off</t>
         </is>
       </c>
-      <c r="I175" t="inlineStr">
-        <is>
-          <t>[0.49764 0.34261 0.4703 ]</t>
-        </is>
+      <c r="I175" t="n">
+        <v>0.7656466655144938</v>
       </c>
       <c r="J175" t="n">
         <v>0.7374751118261998</v>
@@ -8175,10 +7827,8 @@
           <t>testModels/db/4/m406/m406.off</t>
         </is>
       </c>
-      <c r="I176" t="inlineStr">
-        <is>
-          <t>[0.36491 0.26604 0.35223]</t>
-        </is>
+      <c r="I176" t="n">
+        <v>0.5727114092479244</v>
       </c>
       <c r="J176" t="n">
         <v>0.4214042623551</v>
@@ -8219,10 +7869,8 @@
           <t>testModels/db/4/m407/m407.off</t>
         </is>
       </c>
-      <c r="I177" t="inlineStr">
-        <is>
-          <t>[0.41214 0.49648 0.3599 ]</t>
-        </is>
+      <c r="I177" t="n">
+        <v>0.7388373022554811</v>
       </c>
       <c r="J177" t="n">
         <v>0.5377887483226499</v>
@@ -8263,10 +7911,8 @@
           <t>testModels/db/4/m408/m408.off</t>
         </is>
       </c>
-      <c r="I178" t="inlineStr">
-        <is>
-          <t>[0.33435 0.14474 0.52846]</t>
-        </is>
+      <c r="I178" t="n">
+        <v>0.6418806266942023</v>
       </c>
       <c r="J178" t="n">
         <v>0.334412281809</v>
@@ -8307,10 +7953,8 @@
           <t>testModels/db/4/m409/m409.off</t>
         </is>
       </c>
-      <c r="I179" t="inlineStr">
-        <is>
-          <t>[ 0.55001 -0.00152  0.31359]</t>
-        </is>
+      <c r="I179" t="n">
+        <v>0.633128834637152</v>
       </c>
       <c r="J179" t="n">
         <v>0.12750341215795</v>
@@ -8351,10 +7995,8 @@
           <t>testModels/db/4/m410/m410.off</t>
         </is>
       </c>
-      <c r="I180" t="inlineStr">
-        <is>
-          <t>[ 0.50344 -0.39155  0.48966]</t>
-        </is>
+      <c r="I180" t="n">
+        <v>0.8040751622962321</v>
       </c>
       <c r="J180" t="n">
         <v>0.36472700513595</v>
@@ -8395,10 +8037,8 @@
           <t>testModels/db/4/m411/m411.off</t>
         </is>
       </c>
-      <c r="I181" t="inlineStr">
-        <is>
-          <t>[0.47111 0.29202 0.12119]</t>
-        </is>
+      <c r="I181" t="n">
+        <v>0.5673686192841481</v>
       </c>
       <c r="J181" t="n">
         <v>0.2742882714080499</v>
@@ -8439,10 +8079,8 @@
           <t>testModels/db/4/m412/m412.off</t>
         </is>
       </c>
-      <c r="I182" t="inlineStr">
-        <is>
-          <t>[0.52098 0.04239 0.3057 ]</t>
-        </is>
+      <c r="I182" t="n">
+        <v>0.6055354349551082</v>
       </c>
       <c r="J182" t="n">
         <v>0.04766319038249999</v>
@@ -8483,10 +8121,8 @@
           <t>testModels/db/5/m500/m500.off</t>
         </is>
       </c>
-      <c r="I183" t="inlineStr">
-        <is>
-          <t>[0.49232 0.46093 0.3065 ]</t>
-        </is>
+      <c r="I183" t="n">
+        <v>0.740793984655466</v>
       </c>
       <c r="J183" t="n">
         <v>0.774133244696</v>
@@ -8527,10 +8163,8 @@
           <t>testModels/db/5/m501/m501.off</t>
         </is>
       </c>
-      <c r="I184" t="inlineStr">
-        <is>
-          <t>[0.35125 0.43282 0.35123]</t>
-        </is>
+      <c r="I184" t="n">
+        <v>0.6588412181605431</v>
       </c>
       <c r="J184" t="n">
         <v>0.4045155493718</v>
@@ -8571,10 +8205,8 @@
           <t>testModels/db/5/m502/m502.off</t>
         </is>
       </c>
-      <c r="I185" t="inlineStr">
-        <is>
-          <t>[0.35003 0.52918 0.35001]</t>
-        </is>
+      <c r="I185" t="n">
+        <v>0.7246083651851024</v>
       </c>
       <c r="J185" t="n">
         <v>0.4013836450465499</v>
@@ -8615,10 +8247,8 @@
           <t>testModels/db/5/m503/m503.off</t>
         </is>
       </c>
-      <c r="I186" t="inlineStr">
-        <is>
-          <t>[0.45515 0.54141 0.26296]</t>
-        </is>
+      <c r="I186" t="n">
+        <v>0.754608296946927</v>
       </c>
       <c r="J186" t="n">
         <v>0.44607162209075</v>
@@ -8659,10 +8289,8 @@
           <t>testModels/db/5/m504/m504.off</t>
         </is>
       </c>
-      <c r="I187" t="inlineStr">
-        <is>
-          <t>[0.41692 0.31743 0.39763]</t>
-        </is>
+      <c r="I187" t="n">
+        <v>0.657789951852266</v>
       </c>
       <c r="J187" t="n">
         <v>0.50407117646765</v>
@@ -8703,10 +8331,8 @@
           <t>testModels/db/5/m505/m505.off</t>
         </is>
       </c>
-      <c r="I188" t="inlineStr">
-        <is>
-          <t>[0.45747 0.34161 0.5173 ]</t>
-        </is>
+      <c r="I188" t="n">
+        <v>0.7704377465745151</v>
       </c>
       <c r="J188" t="n">
         <v>0.5421435584800499</v>
@@ -8747,10 +8373,8 @@
           <t>testModels/db/5/m506/m506.off</t>
         </is>
       </c>
-      <c r="I189" t="inlineStr">
-        <is>
-          <t>[0.3771  0.16824 0.35383]</t>
-        </is>
+      <c r="I189" t="n">
+        <v>0.5437897527694318</v>
       </c>
       <c r="J189" t="n">
         <v>0.2279900718197999</v>
@@ -8791,10 +8415,8 @@
           <t>testModels/db/5/m507/m507.off</t>
         </is>
       </c>
-      <c r="I190" t="inlineStr">
-        <is>
-          <t>[0.40162 0.23655 0.2912 ]</t>
-        </is>
+      <c r="I190" t="n">
+        <v>0.5495868890426785</v>
       </c>
       <c r="J190" t="n">
         <v>0.41517676746315</v>
@@ -8835,10 +8457,8 @@
           <t>testModels/db/5/m508/m508.off</t>
         </is>
       </c>
-      <c r="I191" t="inlineStr">
-        <is>
-          <t>[0.37656 0.37351 0.32389]</t>
-        </is>
+      <c r="I191" t="n">
+        <v>0.6214631070286883</v>
       </c>
       <c r="J191" t="n">
         <v>0.4471125239474999</v>
@@ -8879,10 +8499,8 @@
           <t>testModels/db/5/m509/m509.off</t>
         </is>
       </c>
-      <c r="I192" t="inlineStr">
-        <is>
-          <t>[0.39358 0.42875 0.36946]</t>
-        </is>
+      <c r="I192" t="n">
+        <v>0.689373729035565</v>
       </c>
       <c r="J192" t="n">
         <v>0.5659933238063999</v>
@@ -8923,10 +8541,8 @@
           <t>testModels/db/5/m510/m510.off</t>
         </is>
       </c>
-      <c r="I193" t="inlineStr">
-        <is>
-          <t>[ 0.31644 -0.37851  0.2736 ]</t>
-        </is>
+      <c r="I193" t="n">
+        <v>0.5641498460595107</v>
       </c>
       <c r="J193" t="n">
         <v>0.2760294710088</v>
@@ -8967,10 +8583,8 @@
           <t>testModels/db/5/m511/m511.off</t>
         </is>
       </c>
-      <c r="I194" t="inlineStr">
-        <is>
-          <t>[0.48776 0.50831 0.66421]</t>
-        </is>
+      <c r="I194" t="n">
+        <v>0.9682295669190819</v>
       </c>
       <c r="J194" t="n">
         <v>0.7889463070987</v>
@@ -9011,10 +8625,8 @@
           <t>testModels/db/5/m512/m512.off</t>
         </is>
       </c>
-      <c r="I195" t="inlineStr">
-        <is>
-          <t>[0.4113  0.324   0.41169]</t>
-        </is>
+      <c r="I195" t="n">
+        <v>0.6660548679857683</v>
       </c>
       <c r="J195" t="n">
         <v>0.56704613894055</v>
@@ -9055,10 +8667,8 @@
           <t>testModels/db/6/m600/m600.off</t>
         </is>
       </c>
-      <c r="I196" t="inlineStr">
-        <is>
-          <t>[0.2576  0.84482 0.46378]</t>
-        </is>
+      <c r="I196" t="n">
+        <v>0.9975832605519875</v>
       </c>
       <c r="J196" t="n">
         <v>0.3289688236004499</v>
@@ -9099,10 +8709,8 @@
           <t>testModels/db/6/m601/m601.off</t>
         </is>
       </c>
-      <c r="I197" t="inlineStr">
-        <is>
-          <t>[0.32694 0.52692 0.36069]</t>
-        </is>
+      <c r="I197" t="n">
+        <v>0.7173779527946508</v>
       </c>
       <c r="J197" t="n">
         <v>0.8049836529864999</v>
@@ -9143,10 +8751,8 @@
           <t>testModels/db/6/m602/m602.off</t>
         </is>
       </c>
-      <c r="I198" t="inlineStr">
-        <is>
-          <t>[0.21671 0.49866 0.45769]</t>
-        </is>
+      <c r="I198" t="n">
+        <v>0.7107106887155397</v>
       </c>
       <c r="J198" t="n">
         <v>0.2173434360375</v>
@@ -9187,10 +8793,8 @@
           <t>testModels/db/6/m603/m603.off</t>
         </is>
       </c>
-      <c r="I199" t="inlineStr">
-        <is>
-          <t>[0.30416 0.49274 0.64283]</t>
-        </is>
+      <c r="I199" t="n">
+        <v>0.8651792668165202</v>
       </c>
       <c r="J199" t="n">
         <v>0.4357544367391</v>
@@ -9231,10 +8835,8 @@
           <t>testModels/db/6/m604/m604.off</t>
         </is>
       </c>
-      <c r="I200" t="inlineStr">
-        <is>
-          <t>[0.24486 0.22149 0.10704]</t>
-        </is>
+      <c r="I200" t="n">
+        <v>0.3470908542920413</v>
       </c>
       <c r="J200" t="n">
         <v>0.083922626992</v>
@@ -9275,10 +8877,8 @@
           <t>testModels/db/6/m605/m605.off</t>
         </is>
       </c>
-      <c r="I201" t="inlineStr">
-        <is>
-          <t>[0.26351 0.19087 0.32873]</t>
-        </is>
+      <c r="I201" t="n">
+        <v>0.4625212177846422</v>
       </c>
       <c r="J201" t="n">
         <v>0.36795691912105</v>
@@ -9319,10 +8919,8 @@
           <t>testModels/db/6/m606/m606.off</t>
         </is>
       </c>
-      <c r="I202" t="inlineStr">
-        <is>
-          <t>[ 0.52206 -0.04326  0.07172]</t>
-        </is>
+      <c r="I202" t="n">
+        <v>0.5287336557623648</v>
       </c>
       <c r="J202" t="n">
         <v>0.3354520743954</v>
@@ -9363,10 +8961,8 @@
           <t>testModels/db/6/m607/m607.off</t>
         </is>
       </c>
-      <c r="I203" t="inlineStr">
-        <is>
-          <t>[0.20979 2.3303  1.84333]</t>
-        </is>
+      <c r="I203" t="n">
+        <v>2.97862239633214</v>
       </c>
       <c r="J203" t="n">
         <v>0.2491597883831999</v>
@@ -9407,10 +9003,8 @@
           <t>testModels/db/6/m608/m608.off</t>
         </is>
       </c>
-      <c r="I204" t="inlineStr">
-        <is>
-          <t>[0.34098 0.08768 0.03102]</t>
-        </is>
+      <c r="I204" t="n">
+        <v>0.3534369058200094</v>
       </c>
       <c r="J204" t="n">
         <v>0.6166739930119999</v>
@@ -9451,10 +9045,8 @@
           <t>testModels/db/6/m609/m609.off</t>
         </is>
       </c>
-      <c r="I205" t="inlineStr">
-        <is>
-          <t>[0.11931 0.15132 0.251  ]</t>
-        </is>
+      <c r="I205" t="n">
+        <v>0.316434615409602</v>
       </c>
       <c r="J205" t="n">
         <v>0.1239595846008</v>
@@ -9495,10 +9087,8 @@
           <t>testModels/db/6/m610/m610.off</t>
         </is>
       </c>
-      <c r="I206" t="inlineStr">
-        <is>
-          <t>[0.4902  0.36764 0.38151]</t>
-        </is>
+      <c r="I206" t="n">
+        <v>0.7218031856560362</v>
       </c>
       <c r="J206" t="n">
         <v>0.3066715312519999</v>
@@ -9539,10 +9129,8 @@
           <t>testModels/db/6/m611/m611.off</t>
         </is>
       </c>
-      <c r="I207" t="inlineStr">
-        <is>
-          <t>[0.6069  0.04979 0.23218]</t>
-        </is>
+      <c r="I207" t="n">
+        <v>0.6517020269898955</v>
       </c>
       <c r="J207" t="n">
         <v>0.337626976131</v>
@@ -9583,10 +9171,8 @@
           <t>testModels/db/6/m612/m612.off</t>
         </is>
       </c>
-      <c r="I208" t="inlineStr">
-        <is>
-          <t>[0.3938  0.197   0.44858]</t>
-        </is>
+      <c r="I208" t="n">
+        <v>0.6285804801766731</v>
       </c>
       <c r="J208" t="n">
         <v>0.6165689174602</v>
@@ -9627,10 +9213,8 @@
           <t>testModels/db/7/m700/m700.off</t>
         </is>
       </c>
-      <c r="I209" t="inlineStr">
-        <is>
-          <t>[0.1467  0.33229 0.06295]</t>
-        </is>
+      <c r="I209" t="n">
+        <v>0.3686454845230034</v>
       </c>
       <c r="J209" t="n">
         <v>0.027180761887565</v>
@@ -9671,10 +9255,8 @@
           <t>testModels/db/7/m701/m701.off</t>
         </is>
       </c>
-      <c r="I210" t="inlineStr">
-        <is>
-          <t>[0.03452 0.166   0.38486]</t>
-        </is>
+      <c r="I210" t="n">
+        <v>0.4205559755155684</v>
       </c>
       <c r="J210" t="n">
         <v>0.005102765082699999</v>
@@ -9715,10 +9297,8 @@
           <t>testModels/db/7/m702/m702.off</t>
         </is>
       </c>
-      <c r="I211" t="inlineStr">
-        <is>
-          <t>[0.07429 0.07428 0.23926]</t>
-        </is>
+      <c r="I211" t="n">
+        <v>0.261309265844208</v>
       </c>
       <c r="J211" t="n">
         <v>0.0092317409798</v>
@@ -9759,10 +9339,8 @@
           <t>testModels/db/7/m703/m703.off</t>
         </is>
       </c>
-      <c r="I212" t="inlineStr">
-        <is>
-          <t>[0.03788 0.07291 0.39827]</t>
-        </is>
+      <c r="I212" t="n">
+        <v>0.4066528654874887</v>
       </c>
       <c r="J212" t="n">
         <v>0.002345430056895</v>
@@ -9803,10 +9381,8 @@
           <t>testModels/db/7/m704/m704.off</t>
         </is>
       </c>
-      <c r="I213" t="inlineStr">
-        <is>
-          <t>[0.04005 0.05927 0.33505]</t>
-        </is>
+      <c r="I213" t="n">
+        <v>0.3426018239453588</v>
       </c>
       <c r="J213" t="n">
         <v>0.001738359126875</v>
@@ -9847,10 +9423,8 @@
           <t>testModels/db/7/m705/m705.off</t>
         </is>
       </c>
-      <c r="I214" t="inlineStr">
-        <is>
-          <t>[0.24593 0.24572 0.05964]</t>
-        </is>
+      <c r="I214" t="n">
+        <v>0.3527274951791061</v>
       </c>
       <c r="J214" t="n">
         <v>0.02916633158573999</v>
@@ -9891,10 +9465,8 @@
           <t>testModels/db/7/m706/m706.off</t>
         </is>
       </c>
-      <c r="I215" t="inlineStr">
-        <is>
-          <t>[ 0.09956 -1.62382 -0.29342]</t>
-        </is>
+      <c r="I215" t="n">
+        <v>1.653113822556624</v>
       </c>
       <c r="J215" t="n">
         <v>0.01502658194752</v>
@@ -9935,10 +9507,8 @@
           <t>testModels/db/7/m707/m707.off</t>
         </is>
       </c>
-      <c r="I216" t="inlineStr">
-        <is>
-          <t>[0.15029 0.32941 0.04555]</t>
-        </is>
+      <c r="I216" t="n">
+        <v>0.3649288564355794</v>
       </c>
       <c r="J216" t="n">
         <v>0.009433590992994999</v>
@@ -9979,10 +9549,8 @@
           <t>testModels/db/7/m708/m708.off</t>
         </is>
       </c>
-      <c r="I217" t="inlineStr">
-        <is>
-          <t>[0.2343  0.67857 0.04457]</t>
-        </is>
+      <c r="I217" t="n">
+        <v>0.7192654525196647</v>
       </c>
       <c r="J217" t="n">
         <v>0.0156089468078</v>
@@ -10023,10 +9591,8 @@
           <t>testModels/db/7/m709/m709.off</t>
         </is>
       </c>
-      <c r="I218" t="inlineStr">
-        <is>
-          <t>[0.12743 0.05072 0.73616]</t>
-        </is>
+      <c r="I218" t="n">
+        <v>0.7488291165068052</v>
       </c>
       <c r="J218" t="n">
         <v>0.01000608285012</v>
@@ -10067,10 +9633,8 @@
           <t>testModels/db/7/m710/m710.off</t>
         </is>
       </c>
-      <c r="I219" t="inlineStr">
-        <is>
-          <t>[0.12764 0.05082 0.55873]</t>
-        </is>
+      <c r="I219" t="n">
+        <v>0.5753770261076903</v>
       </c>
       <c r="J219" t="n">
         <v>0.010036128300715</v>
@@ -10111,10 +9675,8 @@
           <t>testModels/db/7/m711/m711.off</t>
         </is>
       </c>
-      <c r="I220" t="inlineStr">
-        <is>
-          <t>[0.12612 0.04422 0.41518]</t>
-        </is>
+      <c r="I220" t="n">
+        <v>0.4361623866390801</v>
       </c>
       <c r="J220" t="n">
         <v>0.0059225081146</v>
@@ -10155,10 +9717,8 @@
           <t>testModels/db/7/m712/m712.off</t>
         </is>
       </c>
-      <c r="I221" t="inlineStr">
-        <is>
-          <t>[0.6791  0.04682 0.11797]</t>
-        </is>
+      <c r="I221" t="n">
+        <v>0.6908561025698483</v>
       </c>
       <c r="J221" t="n">
         <v>0.0055064394</v>
@@ -10199,10 +9759,8 @@
           <t>testModels/db/8/m800/m800.off</t>
         </is>
       </c>
-      <c r="I222" t="inlineStr">
-        <is>
-          <t>[0.34241 0.611   0.3418 ]</t>
-        </is>
+      <c r="I222" t="n">
+        <v>0.7793533532512145</v>
       </c>
       <c r="J222" t="n">
         <v>0.4692020714198</v>
@@ -10243,10 +9801,8 @@
           <t>testModels/db/8/m801/m801.off</t>
         </is>
       </c>
-      <c r="I223" t="inlineStr">
-        <is>
-          <t>[0.25362 0.53328 0.21781]</t>
-        </is>
+      <c r="I223" t="n">
+        <v>0.6294068538400275</v>
       </c>
       <c r="J223" t="n">
         <v>0.2195227768589999</v>
@@ -10287,10 +9843,8 @@
           <t>testModels/db/8/m802/m802.off</t>
         </is>
       </c>
-      <c r="I224" t="inlineStr">
-        <is>
-          <t>[ 0.29464 -2.5854   0.21186]</t>
-        </is>
+      <c r="I224" t="n">
+        <v>2.610747824521273</v>
       </c>
       <c r="J224" t="n">
         <v>0.4212982889336</v>
@@ -10331,10 +9885,8 @@
           <t>testModels/db/8/m803/m803.off</t>
         </is>
       </c>
-      <c r="I225" t="inlineStr">
-        <is>
-          <t>[0.28753 7.03473 0.74185]</t>
-        </is>
+      <c r="I225" t="n">
+        <v>7.079580740501704</v>
       </c>
       <c r="J225" t="n">
         <v>0.30128957545635</v>
@@ -10375,10 +9927,8 @@
           <t>testModels/db/8/m804/m804.off</t>
         </is>
       </c>
-      <c r="I226" t="inlineStr">
-        <is>
-          <t>[0.36359 0.37657 0.37865]</t>
-        </is>
+      <c r="I226" t="n">
+        <v>0.6460485190928317</v>
       </c>
       <c r="J226" t="n">
         <v>0.4143275475168</v>
@@ -10419,10 +9969,8 @@
           <t>testModels/db/8/m805/m805.off</t>
         </is>
       </c>
-      <c r="I227" t="inlineStr">
-        <is>
-          <t>[0.37738 0.63646 0.29416]</t>
-        </is>
+      <c r="I227" t="n">
+        <v>0.7962567321333174</v>
       </c>
       <c r="J227" t="n">
         <v>0.4718550028118</v>
@@ -10463,10 +10011,8 @@
           <t>testModels/db/8/m806/m806.off</t>
         </is>
       </c>
-      <c r="I228" t="inlineStr">
-        <is>
-          <t>[0.19164 0.54717 0.23847]</t>
-        </is>
+      <c r="I228" t="n">
+        <v>0.6268887507624301</v>
       </c>
       <c r="J228" t="n">
         <v>0.12238963667975</v>
@@ -10507,10 +10053,8 @@
           <t>testModels/db/8/m807/m807.off</t>
         </is>
       </c>
-      <c r="I229" t="inlineStr">
-        <is>
-          <t>[0.215   0.57754 0.14523]</t>
-        </is>
+      <c r="I229" t="n">
+        <v>0.6331449943282442</v>
       </c>
       <c r="J229" t="n">
         <v>0.136760518</v>
@@ -10551,10 +10095,8 @@
           <t>testModels/db/8/m808/m808.off</t>
         </is>
       </c>
-      <c r="I230" t="inlineStr">
-        <is>
-          <t>[ 0.27902 20.89506  2.97992]</t>
-        </is>
+      <c r="I230" t="n">
+        <v>21.10832560523566</v>
       </c>
       <c r="J230" t="n">
         <v>0.29952589509265</v>
@@ -10595,10 +10137,8 @@
           <t>testModels/db/8/m809/m809.off</t>
         </is>
       </c>
-      <c r="I231" t="inlineStr">
-        <is>
-          <t>[0.13359 0.41339 0.08314]</t>
-        </is>
+      <c r="I231" t="n">
+        <v>0.4423214917244146</v>
       </c>
       <c r="J231" t="n">
         <v>0.04148136539820001</v>
@@ -10639,10 +10179,8 @@
           <t>testModels/db/8/m810/m810.off</t>
         </is>
       </c>
-      <c r="I232" t="inlineStr">
-        <is>
-          <t>[0.14771 0.49444 0.21337]</t>
-        </is>
+      <c r="I232" t="n">
+        <v>0.5584035751321208</v>
       </c>
       <c r="J232" t="n">
         <v>0.1273507914384</v>
@@ -10683,10 +10221,8 @@
           <t>testModels/db/8/m811/m811.off</t>
         </is>
       </c>
-      <c r="I233" t="inlineStr">
-        <is>
-          <t>[0.28163 1.02733 0.29182]</t>
-        </is>
+      <c r="I233" t="n">
+        <v>1.104476624916185</v>
       </c>
       <c r="J233" t="n">
         <v>0.2592673744301999</v>
@@ -10727,10 +10263,8 @@
           <t>testModels/db/8/m812/m812.off</t>
         </is>
       </c>
-      <c r="I234" t="inlineStr">
-        <is>
-          <t>[0.24258 1.15872 0.25171]</t>
-        </is>
+      <c r="I234" t="n">
+        <v>1.210301467677619</v>
       </c>
       <c r="J234" t="n">
         <v>0.18636813187305</v>
@@ -10771,10 +10305,8 @@
           <t>testModels/db/9/m900/m900.off</t>
         </is>
       </c>
-      <c r="I235" t="inlineStr">
-        <is>
-          <t>[0.5     0.60787 0.21153]</t>
-        </is>
+      <c r="I235" t="n">
+        <v>0.8150144859999663</v>
       </c>
       <c r="J235" t="n">
         <v>0.2008387393843999</v>
@@ -10815,10 +10347,8 @@
           <t>testModels/db/9/m901/m901.off</t>
         </is>
       </c>
-      <c r="I236" t="inlineStr">
-        <is>
-          <t>[0.49823 0.59489 0.38976]</t>
-        </is>
+      <c r="I236" t="n">
+        <v>0.8683544604370087</v>
       </c>
       <c r="J236" t="n">
         <v>0.4992543045531</v>
@@ -10859,10 +10389,8 @@
           <t>testModels/db/9/m902/m902.off</t>
         </is>
       </c>
-      <c r="I237" t="inlineStr">
-        <is>
-          <t>[0.49915 0.46546 0.23075]</t>
-        </is>
+      <c r="I237" t="n">
+        <v>0.7204514683276981</v>
       </c>
       <c r="J237" t="n">
         <v>0.2234783074855499</v>
@@ -10903,10 +10431,8 @@
           <t>testModels/db/9/m903/m903.off</t>
         </is>
       </c>
-      <c r="I238" t="inlineStr">
-        <is>
-          <t>[0.58441 0.21262 0.13059]</t>
-        </is>
+      <c r="I238" t="n">
+        <v>0.6354507231863391</v>
       </c>
       <c r="J238" t="n">
         <v>0.0451911105855</v>
@@ -10947,10 +10473,8 @@
           <t>testModels/db/9/m904/m904.off</t>
         </is>
       </c>
-      <c r="I239" t="inlineStr">
-        <is>
-          <t>[ 0.21548 -0.29478  0.21548]</t>
-        </is>
+      <c r="I239" t="n">
+        <v>0.4239753447226846</v>
       </c>
       <c r="J239" t="n">
         <v>0.13786748118095</v>
@@ -10991,10 +10515,8 @@
           <t>testModels/db/9/m905/m905.off</t>
         </is>
       </c>
-      <c r="I240" t="inlineStr">
-        <is>
-          <t>[0.49083 1.70803 0.80287]</t>
-        </is>
+      <c r="I240" t="n">
+        <v>1.950102583589145</v>
       </c>
       <c r="J240" t="n">
         <v>0.7364851249999999</v>
@@ -11035,10 +10557,8 @@
           <t>testModels/db/9/m906/m906.off</t>
         </is>
       </c>
-      <c r="I241" t="inlineStr">
-        <is>
-          <t>[0.38697 0.10285 0.51253]</t>
-        </is>
+      <c r="I241" t="n">
+        <v>0.6503986406336092</v>
       </c>
       <c r="J241" t="n">
         <v>0.2187877917004</v>
@@ -11079,10 +10599,8 @@
           <t>testModels/db/9/m907/m907.off</t>
         </is>
       </c>
-      <c r="I242" t="inlineStr">
-        <is>
-          <t>[ 0.24412  3.20385 35.46056]</t>
-        </is>
+      <c r="I242" t="n">
+        <v>35.60583620048602</v>
       </c>
       <c r="J242" t="n">
         <v>0.1806036165228</v>
@@ -11123,10 +10641,8 @@
           <t>testModels/db/9/m908/m908.off</t>
         </is>
       </c>
-      <c r="I243" t="inlineStr">
-        <is>
-          <t>[0.5     0.37471 0.27004]</t>
-        </is>
+      <c r="I243" t="n">
+        <v>0.6806853857961497</v>
       </c>
       <c r="J243" t="n">
         <v>0.1606127350113</v>
@@ -11167,10 +10683,8 @@
           <t>testModels/db/9/m909/m909.off</t>
         </is>
       </c>
-      <c r="I244" t="inlineStr">
-        <is>
-          <t>[0.36429 0.39875 0.5    ]</t>
-        </is>
+      <c r="I244" t="n">
+        <v>0.736009067081599</v>
       </c>
       <c r="J244" t="n">
         <v>0.2699627205685499</v>
@@ -11211,10 +10725,8 @@
           <t>testModels/db/9/m910/m910.off</t>
         </is>
       </c>
-      <c r="I245" t="inlineStr">
-        <is>
-          <t>[1.24503 0.52705 1.56593]</t>
-        </is>
+      <c r="I245" t="n">
+        <v>2.068818970307112</v>
       </c>
       <c r="J245" t="n">
         <v>0.3648737378448</v>
@@ -11255,10 +10767,8 @@
           <t>testModels/db/9/m911/m911.off</t>
         </is>
       </c>
-      <c r="I246" t="inlineStr">
-        <is>
-          <t>[-0.05817 14.26451 -2.7911 ]</t>
-        </is>
+      <c r="I246" t="n">
+        <v>14.53512791946737</v>
       </c>
       <c r="J246" t="n">
         <v>0.20469828125</v>
@@ -11299,10 +10809,8 @@
           <t>testModels/db/9/m912/m912.off</t>
         </is>
       </c>
-      <c r="I247" t="inlineStr">
-        <is>
-          <t>[0.5    0.4696 0.2625]</t>
-        </is>
+      <c r="I247" t="n">
+        <v>0.7344602083317461</v>
       </c>
       <c r="J247" t="n">
         <v>0.21434375</v>

</xml_diff>